<commit_message>
Archivos modificados en estructura del proyecto
</commit_message>
<xml_diff>
--- a/Entregables/Comunicaciones/MAPEO Input Outputs.xlsx
+++ b/Entregables/Comunicaciones/MAPEO Input Outputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Guatemala\2024\POC_HINCAPIE\Entregables\Comunicaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A74FA08-9C56-4F30-92CE-00D51CB87EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419BE651-6C8D-448C-90FA-2A06A84A99BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00DEC3F3-9D5F-4996-ADBB-9228D00EE05E}"/>
   </bookViews>
@@ -683,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -700,7 +700,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1018,7 +1017,7 @@
   <dimension ref="A1:L91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
@@ -4024,8 +4023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5819A573-E956-4915-8A3D-45D54E296554}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K110"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7052,7 +7051,7 @@
       <c r="H109" t="s">
         <v>101</v>
       </c>
-      <c r="I109" s="8" t="s">
+      <c r="I109" t="s">
         <v>165</v>
       </c>
       <c r="K109">
@@ -7117,7 +7116,7 @@
     <col min="12" max="12" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>89</v>
       </c>

</xml_diff>